<commit_message>
add write spare part for week log parts
</commit_message>
<xml_diff>
--- a/eq_log/eq_file/80001111.xlsx
+++ b/eq_log/eq_file/80001111.xlsx
@@ -1,25 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="525" windowWidth="28455" windowHeight="11445"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="main" sheetId="1" r:id="rId1"/>
-    <sheet name="data" sheetId="2" r:id="rId2"/>
+    <sheet name="main" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="data" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="82">
   <si>
     <t>тип обладнання</t>
   </si>
   <si>
+    <t>середне значення циклів між замінами</t>
+  </si>
+  <si>
     <t>дата</t>
   </si>
   <si>
@@ -29,6 +32,9 @@
     <t>причина дефекту/невідповідності</t>
   </si>
   <si>
+    <t>кількість циклів при заміні запчастин</t>
+  </si>
+  <si>
     <t>різниця циклів між замінами</t>
   </si>
   <si>
@@ -101,6 +107,15 @@
     <t>5698</t>
   </si>
   <si>
+    <t>20/02/2018</t>
+  </si>
+  <si>
+    <t>5699</t>
+  </si>
+  <si>
+    <t>5700</t>
+  </si>
+  <si>
     <t>**</t>
   </si>
   <si>
@@ -246,91 +261,86 @@
   </si>
   <si>
     <t>механічне корегування механізмів</t>
-  </si>
-  <si>
-    <t>середне значення циклів між замінами</t>
-  </si>
-  <si>
-    <t>кількість циклів при заміні запчастин</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="9">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <i val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="20"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="20"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="8"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <color rgb="FF006100"/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <charset val="238"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="238"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <charset val="238"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="9"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="238"/>
     </font>
   </fonts>
   <fills count="11">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -343,13 +353,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.1499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="9" tint="0.3999755851924192"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -372,7 +382,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="0.5999938962981048"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -384,7 +394,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
+        <fgColor theme="3" tint="0.7999816888943144"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -554,122 +564,121 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0"/>
+    <xf borderId="0" fillId="6" fontId="6" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="43">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="3" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="5" fontId="2" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="2" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="8" fillId="7" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="9" fillId="7" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="10" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="11" fillId="8" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="8" fillId="9" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="9" fillId="9" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="11" fillId="9" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="8" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="9" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="11" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="6" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="8" fillId="10" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="9" fillId="10" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="11" fillId="10" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="5" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="5" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="3" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="7" fillId="6" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Хороший" xfId="2" builtinId="26"/>
+    <cellStyle builtinId="0" name="Обычный" xfId="0"/>
+    <cellStyle builtinId="8" name="Гиперссылка" xfId="1"/>
+    <cellStyle builtinId="26" name="Хороший" xfId="2"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -957,713 +966,738 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" style="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" style="36" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" style="31" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" style="32" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="32" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="39" width="10.5703125"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="39" width="21"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" style="39" width="34.85546875"/>
+    <col customWidth="1" max="4" min="4" style="40" width="23.7109375"/>
+    <col customWidth="1" max="5" min="5" style="39" width="23.7109375"/>
+    <col customWidth="1" max="6" min="6" style="41" width="23.7109375"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="41" width="11.28515625"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" style="41" width="15.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="38">
+    <row customHeight="1" ht="26.25" r="1" s="41" spans="1:8">
+      <c r="A1" s="38" t="n">
         <v>80001111</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="41"/>
       <c r="G1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="29.45" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="29.45" r="2" s="41" spans="1:8">
       <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="10" t="n"/>
+      <c r="G2" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="37" t="n">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="3" t="n"/>
+      <c r="B3" s="9" t="n"/>
+      <c r="C3" s="2" t="n"/>
+      <c r="D3" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="E3" s="2">
+        <f>D3-D2</f>
+        <v/>
+      </c>
+      <c r="F3" s="11" t="n"/>
+      <c r="G3" s="39" t="n"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="35" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="37">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="3"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="34">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="e">
-        <f t="shared" ref="E3:E24" si="0">D3-D2</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="31"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="35">
-        <v>2</v>
-      </c>
       <c r="E4" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>D4-D3</f>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="35">
+        <v>9</v>
+      </c>
+      <c r="D5" s="35" t="n">
         <v>3</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>D5-D4</f>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="35">
+        <v>9</v>
+      </c>
+      <c r="D6" s="35" t="n">
         <v>4</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>D6-D5</f>
+        <v/>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="35">
+        <v>11</v>
+      </c>
+      <c r="D7" s="35" t="n">
         <v>5</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>D7-D6</f>
+        <v/>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="35">
+        <v>13</v>
+      </c>
+      <c r="D8" s="35" t="n">
         <v>6</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>D8-D7</f>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="35" t="n">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="35">
-        <v>7</v>
-      </c>
       <c r="E9" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>D9-D8</f>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="35">
+        <v>11</v>
+      </c>
+      <c r="D10" s="35" t="n">
         <v>8</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>D10-D9</f>
+        <v/>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="35">
+        <v>18</v>
+      </c>
+      <c r="D11" s="35" t="n">
         <v>9</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>D11-D10</f>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="35">
+        <v>11</v>
+      </c>
+      <c r="D12" s="35" t="n">
         <v>10</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>D12-D11</f>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>D13-D12</f>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" si="0"/>
-        <v>87</v>
+        <f>D14-D13</f>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>D15-D14</f>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="0"/>
-        <v>900</v>
+        <f>D16-D15</f>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>D17-D16</f>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="0"/>
-        <v>4697</v>
+        <f>D18-D17</f>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>31</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" si="0"/>
-        <v>-5698</v>
+        <f>D19-D18</f>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>32</v>
+      </c>
       <c r="E20" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>D20-D19</f>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
       <c r="E21" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>D21-D20</f>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="E22" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>D22-D21</f>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="E23" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>D23-D22</f>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="E24" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>D24-D23</f>
+        <v/>
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="H28" s="1"/>
+      <c r="H28" s="1" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="41.5703125" style="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="32" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="41" width="41.5703125"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="41" width="13.42578125"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" style="41" width="45.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="42"/>
+        <v>11</v>
+      </c>
+      <c r="D1" s="42" t="n"/>
       <c r="E1" s="42" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="2" s="41" spans="1:5" thickBot="1">
       <c r="A2" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="12" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="12" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="12" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="12" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="12" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="12" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="12" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="12" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="12" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="12" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="12" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="17" s="41" spans="1:5" thickBot="1">
       <c r="A17" s="13" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="D18" s="18" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="D19" s="19" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="D20" s="19" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="D21" s="19" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="D22" s="19" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E22" s="24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="23" s="41" spans="1:5" thickBot="1">
+      <c r="D23" s="20" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
-      <c r="D23" s="20" t="s">
-        <v>58</v>
-      </c>
       <c r="E23" s="26" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="D24" s="21" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="D25" s="23" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="D26" s="23" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="27" s="41" spans="1:5" thickBot="1">
       <c r="D27" s="25" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="D28" s="27" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="D29" s="28" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="D30" s="28" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="D31" s="28" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="D32" s="28" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E32" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="33" s="41" spans="1:5" thickBot="1">
+      <c r="D33" s="29" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="33" spans="4:5" ht="15.75" customHeight="1" thickBot="1">
-      <c r="D33" s="29" t="s">
-        <v>70</v>
-      </c>
       <c r="E33" s="26" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1671,6 +1705,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add write spare part to a few file
</commit_message>
<xml_diff>
--- a/eq_log/eq_file/80001111.xlsx
+++ b/eq_log/eq_file/80001111.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="105">
   <si>
     <t>тип обладнання</t>
   </si>
@@ -116,13 +116,82 @@
     <t>5700</t>
   </si>
   <si>
+    <t>21/02/2018</t>
+  </si>
+  <si>
+    <t>5701</t>
+  </si>
+  <si>
+    <t>Гострини на розрізі контакту</t>
+  </si>
+  <si>
+    <t>5702</t>
+  </si>
+  <si>
+    <t>5703</t>
+  </si>
+  <si>
+    <t>5704</t>
+  </si>
+  <si>
+    <t>5705</t>
+  </si>
+  <si>
+    <t>5706</t>
+  </si>
+  <si>
+    <t>5707</t>
+  </si>
+  <si>
+    <t>5708</t>
+  </si>
+  <si>
+    <t>5709</t>
+  </si>
+  <si>
+    <t>5710</t>
+  </si>
+  <si>
+    <t>5711</t>
+  </si>
+  <si>
+    <t>5712</t>
+  </si>
+  <si>
+    <t>5713</t>
+  </si>
+  <si>
+    <t>5714</t>
+  </si>
+  <si>
+    <t>5715</t>
+  </si>
+  <si>
+    <t>5716</t>
+  </si>
+  <si>
+    <t>5717</t>
+  </si>
+  <si>
+    <t>5718</t>
+  </si>
+  <si>
+    <t>5719</t>
+  </si>
+  <si>
+    <t>5720</t>
+  </si>
+  <si>
+    <t>5721</t>
+  </si>
+  <si>
+    <t>5722</t>
+  </si>
+  <si>
     <t>**</t>
   </si>
   <si>
     <t>розшифровка</t>
-  </si>
-  <si>
-    <t>Гострини на розрізі контакту</t>
   </si>
   <si>
     <t>Не симетричне / не відповідне закриття ядра</t>
@@ -971,7 +1040,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -1339,31 +1408,331 @@
       <c r="A21" t="s">
         <v>33</v>
       </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" t="s">
+        <v>34</v>
+      </c>
       <c r="E21" s="2">
         <f>D21-D20</f>
         <v/>
       </c>
     </row>
     <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
+        <v>36</v>
+      </c>
       <c r="E22" s="2">
         <f>D22-D21</f>
         <v/>
       </c>
     </row>
     <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" t="s">
+        <v>37</v>
+      </c>
       <c r="E23" s="2">
         <f>D23-D22</f>
         <v/>
       </c>
     </row>
     <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s">
+        <v>38</v>
+      </c>
       <c r="E24" s="2">
         <f>D24-D23</f>
         <v/>
       </c>
     </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" t="s">
+        <v>41</v>
+      </c>
+    </row>
     <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" t="s">
+        <v>42</v>
+      </c>
       <c r="H28" s="1" t="n"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1399,7 +1768,7 @@
       </c>
       <c r="D1" s="42" t="n"/>
       <c r="E1" s="42" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="2" s="41" spans="1:5" thickBot="1">
@@ -1409,24 +1778,24 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="12" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="12" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1434,10 +1803,10 @@
         <v>28</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1445,43 +1814,43 @@
         <v>18</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="12" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="12" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="12" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1489,65 +1858,65 @@
         <v>14</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="12" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="12" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="12" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="12" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="12" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1555,10 +1924,10 @@
         <v>24</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="17" s="41" spans="1:5" thickBot="1">
@@ -1566,138 +1935,138 @@
         <v>13</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="D18" s="18" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="D19" s="19" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="D20" s="19" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="D21" s="19" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="D22" s="19" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="23" s="41" spans="1:5" thickBot="1">
       <c r="D23" s="20" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="D24" s="21" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="D25" s="23" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="D26" s="23" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="27" s="41" spans="1:5" thickBot="1">
       <c r="D27" s="25" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="D28" s="27" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="D29" s="28" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="D30" s="28" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="D31" s="28" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="D32" s="28" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="E32" s="24" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="33" s="41" spans="1:5" thickBot="1">
       <c r="D33" s="29" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="E33" s="26" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>